<commit_message>
Wrap up work on manuscript v0.2 and start outline and analysis for v0.3
</commit_message>
<xml_diff>
--- a/manuscript/h2_table_single_site_and_eight_site_midwest_and_gulf_subpops_FL50.xlsx
+++ b/manuscript/h2_table_single_site_and_eight_site_midwest_and_gulf_subpops_FL50.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alice\Documents\Github\pvdiv-phenology-gxe\manuscript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FD854362-0CE9-4411-92C8-5F060D7A683B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F08432A0-4D19-4ED9-AE72-928C5BAF46CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595"/>
+    <workbookView xWindow="338" yWindow="487" windowWidth="16875" windowHeight="10530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="h2_table_single_site_and_eight_" sheetId="1" r:id="rId1"/>
@@ -115,10 +115,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="169" formatCode="0.000"/>
-    <numFmt numFmtId="170" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -599,8 +599,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -955,11 +955,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R247"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F37" sqref="F1:G37"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1021,25 +1021,25 @@
         <v>29</v>
       </c>
       <c r="B2" s="1">
-        <v>0.33580239486201002</v>
+        <v>0.81224272052762403</v>
       </c>
       <c r="C2" s="1">
-        <v>7.26575652372317E-2</v>
+        <v>4.7139502185411901E-2</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="G2" s="2">
-        <v>-727.59212242956005</v>
+        <v>2047.4359724994299</v>
       </c>
       <c r="H2" s="2">
-        <v>374.664543816172</v>
+        <v>-1018.68754832832</v>
       </c>
       <c r="L2" s="1">
         <v>5.4289751416243997E-3</v>
@@ -1068,25 +1068,25 @@
         <v>29</v>
       </c>
       <c r="B3" s="1">
-        <v>0.99187732871837697</v>
+        <v>0.9739488425724</v>
       </c>
       <c r="C3" s="1">
-        <v>1.55464203900444E-3</v>
+        <v>4.7229823336854496E-3</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G3" s="2">
-        <v>946.50247316357297</v>
+        <v>3446.4570345500501</v>
       </c>
       <c r="H3" s="2">
-        <v>-467.663987923386</v>
+        <v>-1717.6117461773599</v>
       </c>
       <c r="L3" s="1">
         <v>0.58034666472653695</v>
@@ -1115,25 +1115,25 @@
         <v>29</v>
       </c>
       <c r="B4" s="1">
-        <v>0.85351826725498203</v>
+        <v>0.63207069554096096</v>
       </c>
       <c r="C4" s="1">
-        <v>3.5508766597185798E-2</v>
+        <v>8.3812627881553303E-2</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E4" t="s">
         <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G4" s="2">
-        <v>1261.9706180272899</v>
+        <v>3106.55302238385</v>
       </c>
       <c r="H4" s="2">
-        <v>-625.71745085458497</v>
+        <v>-1547.80424051825</v>
       </c>
       <c r="K4" t="s">
         <v>29</v>
@@ -1259,25 +1259,25 @@
         <v>29</v>
       </c>
       <c r="B7" s="1">
-        <v>0.43145127525508897</v>
+        <v>0.97603116779037602</v>
       </c>
       <c r="C7" s="1">
-        <v>0.17902343319188499</v>
+        <v>8.1467139296658702E-3</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E7" t="s">
         <v>8</v>
       </c>
       <c r="F7" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="G7" s="2">
-        <v>-64.5485428285876</v>
+        <v>468.70218445939901</v>
       </c>
       <c r="H7" s="2">
-        <v>36.762907784025899</v>
+        <v>-230.03360411616299</v>
       </c>
       <c r="K7" t="s">
         <v>29</v>
@@ -1309,25 +1309,25 @@
         <v>29</v>
       </c>
       <c r="B8" s="1">
-        <v>0.88852615394020296</v>
+        <v>0.98691107286079705</v>
       </c>
       <c r="C8" s="1">
-        <v>3.7506855902171198E-2</v>
+        <v>2.3670396246618201E-3</v>
       </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E8" t="s">
         <v>8</v>
       </c>
       <c r="F8" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G8" s="2">
-        <v>624.04297840488005</v>
+        <v>1999.34497217797</v>
       </c>
       <c r="H8" s="2">
-        <v>-307.37709830329902</v>
+        <v>-994.055714991321</v>
       </c>
       <c r="L8" s="1">
         <v>0.54619060849217604</v>
@@ -1356,25 +1356,25 @@
         <v>29</v>
       </c>
       <c r="B9" s="1">
-        <v>0.97603116779037602</v>
+        <v>0.87792031257056402</v>
       </c>
       <c r="C9" s="1">
-        <v>8.1467139296658702E-3</v>
+        <v>3.3797120306543998E-2</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E9" t="s">
         <v>8</v>
       </c>
       <c r="F9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G9" s="2">
-        <v>468.70218445939901</v>
+        <v>1684.12071668149</v>
       </c>
       <c r="H9" s="2">
-        <v>-230.03360411616299</v>
+        <v>-836.58808766707602</v>
       </c>
       <c r="K9" t="s">
         <v>29</v>
@@ -1406,13 +1406,13 @@
         <v>29</v>
       </c>
       <c r="B10" s="1">
-        <v>0.97311208843429198</v>
+        <v>0.99187732871837697</v>
       </c>
       <c r="C10" s="1">
-        <v>9.0097876358369508E-3</v>
+        <v>1.55464203900444E-3</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E10" t="s">
         <v>8</v>
@@ -1421,10 +1421,10 @@
         <v>10</v>
       </c>
       <c r="G10" s="2">
-        <v>299.75891081067999</v>
+        <v>946.50247316357297</v>
       </c>
       <c r="H10" s="2">
-        <v>-145.561967291803</v>
+        <v>-467.663987923386</v>
       </c>
       <c r="K10" t="s">
         <v>29</v>
@@ -1456,25 +1456,25 @@
         <v>29</v>
       </c>
       <c r="B11" s="1">
-        <v>0.90019960940908195</v>
+        <v>0.85351826725498203</v>
       </c>
       <c r="C11" s="1">
-        <v>2.5124218051767899E-2</v>
+        <v>3.5508766597185798E-2</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="E11" t="s">
         <v>8</v>
       </c>
       <c r="F11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G11" s="2">
-        <v>-185.65124247611899</v>
+        <v>1261.9706180272899</v>
       </c>
       <c r="H11" s="2">
-        <v>97.856059159451902</v>
+        <v>-625.71745085458497</v>
       </c>
       <c r="K11" t="s">
         <v>29</v>
@@ -1506,25 +1506,25 @@
         <v>29</v>
       </c>
       <c r="B12" s="1">
-        <v>0.81224272052762403</v>
+        <v>0.88852615394020296</v>
       </c>
       <c r="C12" s="1">
-        <v>4.7139502185411901E-2</v>
+        <v>3.7506855902171198E-2</v>
       </c>
       <c r="D12" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="E12" t="s">
         <v>8</v>
       </c>
       <c r="F12" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G12" s="2">
-        <v>2047.4359724994299</v>
+        <v>624.04297840488005</v>
       </c>
       <c r="H12" s="2">
-        <v>-1018.68754832832</v>
+        <v>-307.37709830329902</v>
       </c>
       <c r="L12" s="1">
         <v>0.60024481889521397</v>
@@ -1553,25 +1553,25 @@
         <v>29</v>
       </c>
       <c r="B13" s="1">
-        <v>0.98691107286079705</v>
+        <v>0.97311208843429198</v>
       </c>
       <c r="C13" s="1">
-        <v>2.3670396246618201E-3</v>
+        <v>9.0097876358369508E-3</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="E13" t="s">
         <v>8</v>
       </c>
       <c r="F13" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G13" s="2">
-        <v>1999.34497217797</v>
+        <v>299.75891081067999</v>
       </c>
       <c r="H13" s="2">
-        <v>-994.055714991321</v>
+        <v>-145.561967291803</v>
       </c>
       <c r="K13" t="s">
         <v>29</v>
@@ -1603,13 +1603,13 @@
         <v>29</v>
       </c>
       <c r="B14" s="1">
-        <v>0.98258864272784396</v>
+        <v>0.33580239486201002</v>
       </c>
       <c r="C14" s="1">
-        <v>3.15177324894643E-3</v>
+        <v>7.26575652372317E-2</v>
       </c>
       <c r="D14" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="E14" t="s">
         <v>8</v>
@@ -1618,10 +1618,10 @@
         <v>9</v>
       </c>
       <c r="G14" s="2">
-        <v>-213.79450881087399</v>
+        <v>-727.59212242956005</v>
       </c>
       <c r="H14" s="2">
-        <v>112.514025503103</v>
+        <v>374.664543816172</v>
       </c>
       <c r="L14" s="1">
         <v>0.50298169777554202</v>
@@ -1650,25 +1650,25 @@
         <v>29</v>
       </c>
       <c r="B15" s="1">
-        <v>0.97695298229148397</v>
+        <v>0.43145127525508897</v>
       </c>
       <c r="C15" s="1">
-        <v>4.1768560811033797E-3</v>
+        <v>0.17902343319188499</v>
       </c>
       <c r="D15" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E15" t="s">
         <v>8</v>
       </c>
       <c r="F15" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G15" s="2">
-        <v>1853.0581499279899</v>
+        <v>-64.5485428285876</v>
       </c>
       <c r="H15" s="2">
-        <v>-920.91230386633003</v>
+        <v>36.762907784025899</v>
       </c>
       <c r="L15" s="1">
         <v>2.2423616200907E-2</v>
@@ -1697,25 +1697,25 @@
         <v>29</v>
       </c>
       <c r="B16" s="1">
-        <v>0.9739488425724</v>
+        <v>0.90019960940908195</v>
       </c>
       <c r="C16" s="1">
-        <v>4.7229823336854496E-3</v>
+        <v>2.5124218051767899E-2</v>
       </c>
       <c r="D16" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="E16" t="s">
         <v>8</v>
       </c>
       <c r="F16" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G16" s="2">
-        <v>3446.4570345500501</v>
+        <v>-185.65124247611899</v>
       </c>
       <c r="H16" s="2">
-        <v>-1717.6117461773599</v>
+        <v>97.856059159451902</v>
       </c>
       <c r="K16" t="s">
         <v>29</v>
@@ -1747,25 +1747,25 @@
         <v>29</v>
       </c>
       <c r="B17" s="1">
-        <v>0.87792031257056402</v>
+        <v>0.98258864272784396</v>
       </c>
       <c r="C17" s="1">
-        <v>3.3797120306543998E-2</v>
+        <v>3.15177324894643E-3</v>
       </c>
       <c r="D17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E17" t="s">
         <v>8</v>
       </c>
       <c r="F17" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G17" s="2">
-        <v>1684.12071668149</v>
+        <v>-213.79450881087399</v>
       </c>
       <c r="H17" s="2">
-        <v>-836.58808766707602</v>
+        <v>112.514025503103</v>
       </c>
       <c r="L17" s="1">
         <v>0.68944077959566996</v>
@@ -1844,25 +1844,25 @@
         <v>29</v>
       </c>
       <c r="B19" s="1">
-        <v>0.63207069554096096</v>
+        <v>0.97695298229148397</v>
       </c>
       <c r="C19" s="1">
-        <v>8.3812627881553303E-2</v>
+        <v>4.1768560811033797E-3</v>
       </c>
       <c r="D19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E19" t="s">
         <v>8</v>
       </c>
       <c r="F19" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G19" s="2">
-        <v>3106.55302238385</v>
+        <v>1853.0581499279899</v>
       </c>
       <c r="H19" s="2">
-        <v>-1547.80424051825</v>
+        <v>-920.91230386633003</v>
       </c>
       <c r="K19" t="s">
         <v>29</v>
@@ -1894,10 +1894,10 @@
         <v>29</v>
       </c>
       <c r="B20" s="1">
-        <v>0.99954167880964495</v>
+        <v>0.95382854411687901</v>
       </c>
       <c r="C20" s="1">
-        <v>1.5157443683079699E-3</v>
+        <v>1.9623865117708701E-2</v>
       </c>
       <c r="D20" t="s">
         <v>28</v>
@@ -1906,13 +1906,13 @@
         <v>27</v>
       </c>
       <c r="F20" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G20" s="2">
-        <v>22849.8039217402</v>
+        <v>11855.2775716715</v>
       </c>
       <c r="H20" s="2">
-        <v>-11417.2911080797</v>
+        <v>-5920.0279330453504</v>
       </c>
       <c r="L20" s="1">
         <v>2.07009932789399E-2</v>
@@ -1941,10 +1941,10 @@
         <v>29</v>
       </c>
       <c r="B21" s="1">
-        <v>0.98963645139455103</v>
+        <v>0.94833243177159399</v>
       </c>
       <c r="C21" s="1">
-        <v>6.74033065857064E-3</v>
+        <v>1.9304010454408601E-2</v>
       </c>
       <c r="D21" t="s">
         <v>28</v>
@@ -1953,13 +1953,13 @@
         <v>27</v>
       </c>
       <c r="F21" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G21" s="2">
-        <v>15000.099655182599</v>
+        <v>12536.0505988856</v>
       </c>
       <c r="H21" s="2">
-        <v>-7492.4389748008998</v>
+        <v>-6260.4144466524303</v>
       </c>
       <c r="L21" s="1">
         <v>1.7656097843282401E-6</v>
@@ -1988,10 +1988,10 @@
         <v>29</v>
       </c>
       <c r="B22" s="1">
-        <v>0.95382854411687901</v>
+        <v>0.98963645139455103</v>
       </c>
       <c r="C22" s="1">
-        <v>1.9623865117708701E-2</v>
+        <v>6.74033065857064E-3</v>
       </c>
       <c r="D22" t="s">
         <v>28</v>
@@ -2000,13 +2000,13 @@
         <v>27</v>
       </c>
       <c r="F22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G22" s="2">
-        <v>11855.2775716715</v>
+        <v>15000.099655182599</v>
       </c>
       <c r="H22" s="2">
-        <v>-5920.0279330453504</v>
+        <v>-7492.4389748008998</v>
       </c>
       <c r="K22" t="s">
         <v>29</v>
@@ -2038,10 +2038,10 @@
         <v>29</v>
       </c>
       <c r="B23" s="1">
-        <v>0.94833243177159399</v>
+        <v>0.99954167880964495</v>
       </c>
       <c r="C23" s="1">
-        <v>1.9304010454408601E-2</v>
+        <v>1.5157443683079699E-3</v>
       </c>
       <c r="D23" t="s">
         <v>28</v>
@@ -2050,13 +2050,13 @@
         <v>27</v>
       </c>
       <c r="F23" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G23" s="2">
-        <v>12536.0505988856</v>
+        <v>22849.8039217402</v>
       </c>
       <c r="H23" s="2">
-        <v>-6260.4144466524303</v>
+        <v>-11417.2911080797</v>
       </c>
       <c r="L23" s="1">
         <v>7.4872810141106297E-7</v>
@@ -2085,10 +2085,10 @@
         <v>29</v>
       </c>
       <c r="B24" s="1">
-        <v>0.94755693570673505</v>
+        <v>0.93037758484724797</v>
       </c>
       <c r="C24" s="1">
-        <v>1.18747372408153E-2</v>
+        <v>1.50865772620325E-2</v>
       </c>
       <c r="D24" t="s">
         <v>28</v>
@@ -2097,13 +2097,13 @@
         <v>27</v>
       </c>
       <c r="F24" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G24" s="2">
-        <v>19104.085909871501</v>
+        <v>21954.546732815001</v>
       </c>
       <c r="H24" s="2">
-        <v>-9544.4321021453707</v>
+        <v>-10969.662513617101</v>
       </c>
       <c r="K24" t="s">
         <v>29</v>
@@ -2135,10 +2135,10 @@
         <v>29</v>
       </c>
       <c r="B25" s="1">
-        <v>0.93037758484724797</v>
+        <v>0.94755693570673505</v>
       </c>
       <c r="C25" s="1">
-        <v>1.50865772620325E-2</v>
+        <v>1.18747372408153E-2</v>
       </c>
       <c r="D25" t="s">
         <v>28</v>
@@ -2147,13 +2147,13 @@
         <v>27</v>
       </c>
       <c r="F25" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G25" s="2">
-        <v>21954.546732815001</v>
+        <v>19104.085909871501</v>
       </c>
       <c r="H25" s="2">
-        <v>-10969.662513617101</v>
+        <v>-9544.4321021453707</v>
       </c>
       <c r="K25" t="s">
         <v>29</v>
@@ -7473,8 +7473,9 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A28:H43">
-    <sortCondition ref="F30"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H25">
+    <sortCondition ref="E2:E25"/>
+    <sortCondition ref="F2:F25"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>